<commit_message>
Basedata import: Skip spreadsheet rows with blank or NA coord values
Fixes #691
</commit_message>
<xml_diff>
--- a/t/test_spreadsheet_import_dms_coords.xlsx
+++ b/t/test_spreadsheet_import_dms_coords.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="22">
   <si>
     <t>num</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>134° 30' 22' E</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>43° 32' 37" S</t>
+  </si>
+  <si>
+    <t>154° 30' 22' E</t>
   </si>
 </sst>
 </file>
@@ -565,9 +574,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E12" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -929,7 +941,7 @@
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -946,7 +958,7 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -963,7 +975,7 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -980,7 +992,7 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -997,7 +1009,7 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1014,7 +1026,7 @@
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1031,7 +1043,7 @@
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1048,7 +1060,7 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1065,8 +1077,40 @@
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>